<commit_message>
try grid search for svm
</commit_message>
<xml_diff>
--- a/models/class_errors.xlsx
+++ b/models/class_errors.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\PredictingRatings\models\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
   <si>
     <t>Группа</t>
   </si>
@@ -76,8 +81,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,17 +141,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -184,9 +197,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,9 +231,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,9 +266,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,14 +442,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -462,13 +483,13 @@
         <v>1150192.575</v>
       </c>
       <c r="D2">
-        <v>134.936</v>
+        <v>134.93600000000001</v>
       </c>
       <c r="E2">
-        <v>168.908</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>168.90799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -476,16 +497,16 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>1566282.369</v>
+        <v>1566282.3689999999</v>
       </c>
       <c r="D3">
-        <v>95.28400000000001</v>
+        <v>95.284000000000006</v>
       </c>
       <c r="E3">
         <v>117.437</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -493,16 +514,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1127526.174</v>
+        <v>1127526.1740000001</v>
       </c>
       <c r="D4">
-        <v>94.559</v>
+        <v>94.558999999999997</v>
       </c>
       <c r="E4">
         <v>115.893</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -513,13 +534,13 @@
         <v>1099642.476</v>
       </c>
       <c r="D5">
-        <v>94.601</v>
+        <v>94.600999999999999</v>
       </c>
       <c r="E5">
         <v>116.295</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -527,7 +548,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1235910.8985</v>
+        <v>1235910.8984999999</v>
       </c>
       <c r="D6">
         <v>104.845</v>
@@ -536,7 +557,7 @@
         <v>129.63325</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -544,16 +565,16 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>404246.543</v>
+        <v>404246.54300000001</v>
       </c>
       <c r="D7">
-        <v>158.032</v>
+        <v>158.03200000000001</v>
       </c>
       <c r="E7">
-        <v>195.802</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>195.80199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -561,16 +582,16 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>3344622.109</v>
+        <v>3344622.1090000002</v>
       </c>
       <c r="D8">
-        <v>678.147</v>
+        <v>678.14700000000005</v>
       </c>
       <c r="E8">
-        <v>893.174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>893.17399999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -578,16 +599,16 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>357067.155</v>
+        <v>357067.15500000003</v>
       </c>
       <c r="D9">
-        <v>99.795</v>
+        <v>99.795000000000002</v>
       </c>
       <c r="E9">
-        <v>122.906</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>122.90600000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -595,7 +616,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>353996.543</v>
+        <v>353996.54300000001</v>
       </c>
       <c r="D10">
         <v>101.49</v>
@@ -604,7 +625,7 @@
         <v>125.63</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -612,16 +633,16 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>1114983.0875</v>
+        <v>1114983.0874999999</v>
       </c>
       <c r="D11">
-        <v>259.366</v>
+        <v>259.36599999999999</v>
       </c>
       <c r="E11">
-        <v>334.3779999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>334.37799999999987</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -629,16 +650,16 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>487078.144</v>
+        <v>487078.14399999997</v>
       </c>
       <c r="D12">
-        <v>190.414</v>
+        <v>190.41399999999999</v>
       </c>
       <c r="E12">
-        <v>246.692</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>246.69200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -646,16 +667,16 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>3521218.942</v>
+        <v>3521218.9419999998</v>
       </c>
       <c r="D13">
-        <v>713.954</v>
+        <v>713.95399999999995</v>
       </c>
       <c r="E13">
         <v>934.84</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -672,7 +693,7 @@
         <v>126.696</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -680,7 +701,7 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>364011.142</v>
+        <v>364011.14199999999</v>
       </c>
       <c r="D15">
         <v>104.361</v>
@@ -689,7 +710,7 @@
         <v>128.952</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -697,16 +718,16 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>1184766.8345</v>
+        <v>1184766.8345000001</v>
       </c>
       <c r="D16">
-        <v>277.80825</v>
+        <v>277.80824999999999</v>
       </c>
       <c r="E16">
-        <v>359.295</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>359.29500000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -714,16 +735,16 @@
         <v>14</v>
       </c>
       <c r="C17">
-        <v>422595.078</v>
+        <v>422595.07799999998</v>
       </c>
       <c r="D17">
-        <v>165.205</v>
+        <v>165.20500000000001</v>
       </c>
       <c r="E17">
-        <v>204.978</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>204.97800000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -731,16 +752,16 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <v>3367924.717</v>
+        <v>3367924.7170000002</v>
       </c>
       <c r="D18">
-        <v>682.872</v>
+        <v>682.87199999999996</v>
       </c>
       <c r="E18">
-        <v>897.579</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>897.57899999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -754,10 +775,10 @@
         <v>102.74</v>
       </c>
       <c r="E19">
-        <v>126.272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>126.27200000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -765,16 +786,16 @@
         <v>14</v>
       </c>
       <c r="C20">
-        <v>362853.118</v>
+        <v>362853.11800000002</v>
       </c>
       <c r="D20">
         <v>104.029</v>
       </c>
       <c r="E20">
-        <v>128.158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>128.15799999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -788,432 +809,347 @@
         <v>263.7115</v>
       </c>
       <c r="E21">
-        <v>339.24675</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>339.24675000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22">
-        <v>471408.969</v>
+        <v>390673.19099999999</v>
       </c>
       <c r="D22">
-        <v>184.288</v>
+        <v>152.726</v>
       </c>
       <c r="E22">
-        <v>231.231</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>193.32599999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23">
-        <v>3390597.785</v>
+        <v>3269403.99</v>
       </c>
       <c r="D23">
-        <v>687.4690000000001</v>
+        <v>662.89599999999996</v>
       </c>
       <c r="E23">
-        <v>897.822</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>873.15099999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24">
-        <v>415609.899</v>
+        <v>353735.94799999997</v>
       </c>
       <c r="D24">
-        <v>116.157</v>
+        <v>98.864000000000004</v>
       </c>
       <c r="E24">
-        <v>144.317</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>121.666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <v>420643.771</v>
+        <v>349644.51400000002</v>
       </c>
       <c r="D25">
-        <v>120.597</v>
+        <v>100.242</v>
       </c>
       <c r="E25">
-        <v>150.048</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>124.08</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26">
-        <v>1174565.106</v>
+        <v>1090864.41075</v>
       </c>
       <c r="D26">
-        <v>277.12775</v>
+        <v>253.68199999999999</v>
       </c>
       <c r="E26">
-        <v>355.8545</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>328.05574999999988</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>390673.191</v>
+        <v>471408.96899999998</v>
       </c>
       <c r="D27">
-        <v>152.726</v>
+        <v>184.28800000000001</v>
       </c>
       <c r="E27">
-        <v>193.326</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>231.23099999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>3269403.99</v>
+        <v>3390597.7850000001</v>
       </c>
       <c r="D28">
-        <v>662.896</v>
+        <v>687.46900000000005</v>
       </c>
       <c r="E28">
-        <v>873.151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>897.822</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>353735.948</v>
+        <v>415609.89899999998</v>
       </c>
       <c r="D29">
-        <v>98.864</v>
+        <v>116.157</v>
       </c>
       <c r="E29">
-        <v>121.666</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>144.31700000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30">
-        <v>349644.514</v>
+        <v>420643.77100000001</v>
       </c>
       <c r="D30">
-        <v>100.242</v>
+        <v>120.59699999999999</v>
       </c>
       <c r="E30">
-        <v>124.08</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>150.048</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>1090864.41075</v>
+        <v>1174565.1059999999</v>
       </c>
       <c r="D31">
-        <v>253.682</v>
+        <v>277.12774999999999</v>
       </c>
       <c r="E31">
-        <v>328.0557499999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>355.85449999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C32">
-        <v>471408.969</v>
+        <v>530705.20200000005</v>
       </c>
       <c r="D32">
-        <v>184.288</v>
+        <v>207.46899999999999</v>
       </c>
       <c r="E32">
-        <v>231.231</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>262.47500000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>3390597.785</v>
+        <v>3476440.5720000002</v>
       </c>
       <c r="D33">
-        <v>687.4690000000001</v>
+        <v>704.87400000000002</v>
       </c>
       <c r="E33">
-        <v>897.822</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>907.80399999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C34">
-        <v>415609.899</v>
+        <v>636832.83499999996</v>
       </c>
       <c r="D34">
-        <v>116.157</v>
+        <v>177.98599999999999</v>
       </c>
       <c r="E34">
-        <v>144.317</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>236.03299999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C35">
-        <v>420643.771</v>
+        <v>846543.022</v>
       </c>
       <c r="D35">
-        <v>120.597</v>
+        <v>242.702</v>
       </c>
       <c r="E35">
-        <v>150.048</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>2524.9670000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C36">
-        <v>1174565.106</v>
+        <v>1372630.40775</v>
       </c>
       <c r="D36">
-        <v>277.12775</v>
+        <v>333.25774999999999</v>
       </c>
       <c r="E36">
-        <v>355.8545</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>982.81975</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C37">
-        <v>530705.202</v>
+        <v>4751046</v>
       </c>
       <c r="D37">
-        <v>207.469</v>
+        <v>1857.328</v>
       </c>
       <c r="E37">
-        <v>262.475</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>1895.49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C38">
-        <v>3476440.572</v>
+        <v>12308305.698000001</v>
       </c>
       <c r="D38">
-        <v>704.874</v>
+        <v>2495.6010000000001</v>
       </c>
       <c r="E38">
-        <v>907.804</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>2501.703</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C39">
-        <v>636832.835</v>
+        <v>7872189</v>
       </c>
       <c r="D39">
-        <v>177.986</v>
+        <v>2200.165</v>
       </c>
       <c r="E39">
-        <v>236.033</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>2210.16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C40">
-        <v>846543.022</v>
+        <v>7715749</v>
       </c>
       <c r="D40">
-        <v>242.702</v>
+        <v>2212.0839999999998</v>
       </c>
       <c r="E40">
-        <v>2524.967</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>2223.7469999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C41">
-        <v>1372630.40775</v>
+        <v>8161822.4244999997</v>
       </c>
       <c r="D41">
-        <v>333.25775</v>
+        <v>2191.2945</v>
       </c>
       <c r="E41">
-        <v>982.81975</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42">
-        <v>4751046</v>
-      </c>
-      <c r="D42">
-        <v>1857.328</v>
-      </c>
-      <c r="E42">
-        <v>1895.49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43">
-        <v>12308305.698</v>
-      </c>
-      <c r="D43">
-        <v>2495.601</v>
-      </c>
-      <c r="E43">
-        <v>2501.703</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" t="s">
-        <v>18</v>
-      </c>
-      <c r="C44">
-        <v>7872189</v>
-      </c>
-      <c r="D44">
-        <v>2200.165</v>
-      </c>
-      <c r="E44">
-        <v>2210.16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45">
-        <v>7715749</v>
-      </c>
-      <c r="D45">
-        <v>2212.084</v>
-      </c>
-      <c r="E45">
-        <v>2223.747</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46">
-        <v>8161822.4245</v>
-      </c>
-      <c r="D46">
-        <v>2191.2945</v>
-      </c>
-      <c r="E46">
-        <v>2207.775</v>
+        <v>2207.7750000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
voting regressor by cluster
</commit_message>
<xml_diff>
--- a/models/class_errors.xlsx
+++ b/models/class_errors.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\PredictingRatings\models\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="20">
   <si>
     <t>Группа</t>
   </si>
@@ -66,23 +61,26 @@
     <t>Extra Trees</t>
   </si>
   <si>
+    <t>SVM</t>
+  </si>
+  <si>
     <t>K-Neighbors</t>
   </si>
   <si>
-    <t>SVM</t>
-  </si>
-  <si>
     <t>ElasticNet</t>
   </si>
   <si>
     <t>XGBoost</t>
+  </si>
+  <si>
+    <t>Voting Regressor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,25 +139,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,9 +187,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,10 +221,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,10 +255,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -442,20 +430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -483,13 +465,13 @@
         <v>1150192.575</v>
       </c>
       <c r="D2">
-        <v>134.93600000000001</v>
+        <v>134.936</v>
       </c>
       <c r="E2">
-        <v>168.90799999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>168.908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -497,16 +479,16 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>1566282.3689999999</v>
+        <v>1566282.369</v>
       </c>
       <c r="D3">
-        <v>95.284000000000006</v>
+        <v>95.28400000000001</v>
       </c>
       <c r="E3">
         <v>117.437</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -514,16 +496,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1127526.1740000001</v>
+        <v>1127526.174</v>
       </c>
       <c r="D4">
-        <v>94.558999999999997</v>
+        <v>94.559</v>
       </c>
       <c r="E4">
         <v>115.893</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -534,13 +516,13 @@
         <v>1099642.476</v>
       </c>
       <c r="D5">
-        <v>94.600999999999999</v>
+        <v>94.601</v>
       </c>
       <c r="E5">
         <v>116.295</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -548,7 +530,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1235910.8984999999</v>
+        <v>1235910.8985</v>
       </c>
       <c r="D6">
         <v>104.845</v>
@@ -557,7 +539,7 @@
         <v>129.63325</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -565,16 +547,16 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>404246.54300000001</v>
+        <v>404246.543</v>
       </c>
       <c r="D7">
-        <v>158.03200000000001</v>
+        <v>158.032</v>
       </c>
       <c r="E7">
-        <v>195.80199999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>195.802</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -582,16 +564,16 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>3344622.1090000002</v>
+        <v>3344622.109</v>
       </c>
       <c r="D8">
-        <v>678.14700000000005</v>
+        <v>678.147</v>
       </c>
       <c r="E8">
-        <v>893.17399999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>893.174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -599,16 +581,16 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>357067.15500000003</v>
+        <v>357067.155</v>
       </c>
       <c r="D9">
-        <v>99.795000000000002</v>
+        <v>99.795</v>
       </c>
       <c r="E9">
-        <v>122.90600000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122.906</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -616,7 +598,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>353996.54300000001</v>
+        <v>353996.543</v>
       </c>
       <c r="D10">
         <v>101.49</v>
@@ -625,7 +607,7 @@
         <v>125.63</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -633,16 +615,16 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>1114983.0874999999</v>
+        <v>1114983.0875</v>
       </c>
       <c r="D11">
-        <v>259.36599999999999</v>
+        <v>259.366</v>
       </c>
       <c r="E11">
-        <v>334.37799999999987</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>334.3779999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -650,16 +632,16 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>487078.14399999997</v>
+        <v>487078.144</v>
       </c>
       <c r="D12">
-        <v>190.41399999999999</v>
+        <v>190.414</v>
       </c>
       <c r="E12">
-        <v>246.69200000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>246.692</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -667,16 +649,16 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>3521218.9419999998</v>
+        <v>3521218.942</v>
       </c>
       <c r="D13">
-        <v>713.95399999999995</v>
+        <v>713.954</v>
       </c>
       <c r="E13">
         <v>934.84</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -693,7 +675,7 @@
         <v>126.696</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -701,7 +683,7 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>364011.14199999999</v>
+        <v>364011.142</v>
       </c>
       <c r="D15">
         <v>104.361</v>
@@ -710,7 +692,7 @@
         <v>128.952</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -718,16 +700,16 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>1184766.8345000001</v>
+        <v>1184766.8345</v>
       </c>
       <c r="D16">
-        <v>277.80824999999999</v>
+        <v>277.80825</v>
       </c>
       <c r="E16">
-        <v>359.29500000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>359.295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -735,16 +717,16 @@
         <v>14</v>
       </c>
       <c r="C17">
-        <v>422595.07799999998</v>
+        <v>422595.078</v>
       </c>
       <c r="D17">
-        <v>165.20500000000001</v>
+        <v>165.205</v>
       </c>
       <c r="E17">
-        <v>204.97800000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204.978</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -752,16 +734,16 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <v>3367924.7170000002</v>
+        <v>3367924.717</v>
       </c>
       <c r="D18">
-        <v>682.87199999999996</v>
+        <v>682.872</v>
       </c>
       <c r="E18">
-        <v>897.57899999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>897.579</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -775,10 +757,10 @@
         <v>102.74</v>
       </c>
       <c r="E19">
-        <v>126.27200000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>126.272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -786,16 +768,16 @@
         <v>14</v>
       </c>
       <c r="C20">
-        <v>362853.11800000002</v>
+        <v>362853.118</v>
       </c>
       <c r="D20">
         <v>104.029</v>
       </c>
       <c r="E20">
-        <v>128.15799999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128.158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -809,69 +791,69 @@
         <v>263.7115</v>
       </c>
       <c r="E21">
-        <v>339.24675000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>339.24675</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>390673.19099999999</v>
+        <v>390673.191</v>
       </c>
       <c r="D22">
         <v>152.726</v>
       </c>
       <c r="E22">
-        <v>193.32599999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>193.326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <v>3269403.99</v>
       </c>
       <c r="D23">
-        <v>662.89599999999996</v>
+        <v>662.896</v>
       </c>
       <c r="E23">
-        <v>873.15099999999995</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>873.151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24">
-        <v>353735.94799999997</v>
+        <v>353735.948</v>
       </c>
       <c r="D24">
-        <v>98.864000000000004</v>
+        <v>98.864</v>
       </c>
       <c r="E24">
         <v>121.666</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25">
-        <v>349644.51400000002</v>
+        <v>349644.514</v>
       </c>
       <c r="D25">
         <v>100.242</v>
@@ -880,109 +862,109 @@
         <v>124.08</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26">
         <v>1090864.41075</v>
       </c>
       <c r="D26">
-        <v>253.68199999999999</v>
+        <v>253.682</v>
       </c>
       <c r="E26">
-        <v>328.05574999999988</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>328.0557499999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27">
-        <v>471408.96899999998</v>
+        <v>471408.969</v>
       </c>
       <c r="D27">
-        <v>184.28800000000001</v>
+        <v>184.288</v>
       </c>
       <c r="E27">
-        <v>231.23099999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>231.231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>3390597.7850000001</v>
+        <v>3390597.785</v>
       </c>
       <c r="D28">
-        <v>687.46900000000005</v>
+        <v>687.4690000000001</v>
       </c>
       <c r="E28">
         <v>897.822</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>415609.89899999998</v>
+        <v>415609.899</v>
       </c>
       <c r="D29">
         <v>116.157</v>
       </c>
       <c r="E29">
-        <v>144.31700000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144.317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <v>420643.77100000001</v>
+        <v>420643.771</v>
       </c>
       <c r="D30">
-        <v>120.59699999999999</v>
+        <v>120.597</v>
       </c>
       <c r="E30">
         <v>150.048</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C31">
-        <v>1174565.1059999999</v>
+        <v>1174565.106</v>
       </c>
       <c r="D31">
-        <v>277.12774999999999</v>
+        <v>277.12775</v>
       </c>
       <c r="E31">
-        <v>355.85449999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>355.8545</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -990,16 +972,16 @@
         <v>17</v>
       </c>
       <c r="C32">
-        <v>530705.20200000005</v>
+        <v>530705.202</v>
       </c>
       <c r="D32">
-        <v>207.46899999999999</v>
+        <v>207.469</v>
       </c>
       <c r="E32">
-        <v>262.47500000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>262.475</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1007,16 +989,16 @@
         <v>17</v>
       </c>
       <c r="C33">
-        <v>3476440.5720000002</v>
+        <v>3476440.572</v>
       </c>
       <c r="D33">
-        <v>704.87400000000002</v>
+        <v>704.874</v>
       </c>
       <c r="E33">
-        <v>907.80399999999997</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>907.804</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1024,16 +1006,16 @@
         <v>17</v>
       </c>
       <c r="C34">
-        <v>636832.83499999996</v>
+        <v>636832.835</v>
       </c>
       <c r="D34">
-        <v>177.98599999999999</v>
+        <v>177.986</v>
       </c>
       <c r="E34">
-        <v>236.03299999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>236.033</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1047,10 +1029,10 @@
         <v>242.702</v>
       </c>
       <c r="E35">
-        <v>2524.9670000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2524.967</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1061,13 +1043,13 @@
         <v>1372630.40775</v>
       </c>
       <c r="D36">
-        <v>333.25774999999999</v>
+        <v>333.25775</v>
       </c>
       <c r="E36">
         <v>982.81975</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1084,7 +1066,7 @@
         <v>1895.49</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1092,16 +1074,16 @@
         <v>18</v>
       </c>
       <c r="C38">
-        <v>12308305.698000001</v>
+        <v>12308305.698</v>
       </c>
       <c r="D38">
-        <v>2495.6010000000001</v>
+        <v>2495.601</v>
       </c>
       <c r="E38">
         <v>2501.703</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1100,7 @@
         <v>2210.16</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1129,13 +1111,13 @@
         <v>7715749</v>
       </c>
       <c r="D40">
-        <v>2212.0839999999998</v>
+        <v>2212.084</v>
       </c>
       <c r="E40">
-        <v>2223.7469999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2223.747</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1143,13 +1125,98 @@
         <v>18</v>
       </c>
       <c r="C41">
-        <v>8161822.4244999997</v>
+        <v>8161822.4245</v>
       </c>
       <c r="D41">
         <v>2191.2945</v>
       </c>
       <c r="E41">
-        <v>2207.7750000000001</v>
+        <v>2207.775</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42">
+        <v>399518.698</v>
+      </c>
+      <c r="D42">
+        <v>156.184</v>
+      </c>
+      <c r="E42">
+        <v>194.666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43">
+        <v>3317708.983</v>
+      </c>
+      <c r="D43">
+        <v>672.6900000000001</v>
+      </c>
+      <c r="E43">
+        <v>886.073</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44">
+        <v>356251.702</v>
+      </c>
+      <c r="D44">
+        <v>99.56699999999999</v>
+      </c>
+      <c r="E44">
+        <v>122.565</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45">
+        <v>357349.805</v>
+      </c>
+      <c r="D45">
+        <v>102.451</v>
+      </c>
+      <c r="E45">
+        <v>140.178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46">
+        <v>1107707.297</v>
+      </c>
+      <c r="D46">
+        <v>257.723</v>
+      </c>
+      <c r="E46">
+        <v>335.8705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>